<commit_message>
Update graph in Sep 0.10.0 - 21 GB/s CSV Parsing Using SIMD on AMD 9950X 🚀
</commit_message>
<xml_diff>
--- a/images/2025-05-sep-0.10.0/sep-perf-0.1.0-to-0.10.0.xlsx
+++ b/images/2025-05-sep-0.10.0/sep-perf-0.1.0-to-0.10.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\oss\nietras.github.io\images\2025-04-sep-0.10.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\oss\nietras.github.io\images\2025-05-sep-0.10.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3CBC92-2054-4A3B-AD46-5311E6513306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACD6FA6-A64A-4EE5-A86D-9257DE07B4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,6 +195,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7CAFDE"/>
       <color rgb="FFC198E0"/>
       <color rgb="FFB482DA"/>
     </mruColors>
@@ -1473,12 +1474,63 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
+      <cdr:x>0.7828</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78499</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA92422-2B5F-8441-9152-04C287BCECF4}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="5559700" y="0"/>
+          <a:ext cx="15530" cy="4949895"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
       <cdr:x>0.29446</cdr:x>
       <cdr:y>0.02196</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.7121</cdr:x>
-      <cdr:y>0.28199</cdr:y>
+      <cdr:y>0.30119</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1493,8 +1545,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2091358" y="108710"/>
-          <a:ext cx="2966210" cy="1287117"/>
+          <a:off x="2091354" y="108700"/>
+          <a:ext cx="2966219" cy="1382170"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1543,9 +1595,186 @@
             </a:rPr>
             <a:t>Performance Progression</a:t>
           </a:r>
-          <a:endParaRPr lang="en-DK" sz="2000" kern="1200">
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C198E0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Across Different Sep &amp; .NET Versions and CPUs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-DK" sz="1100" kern="1200">
             <a:solidFill>
               <a:srgbClr val="C198E0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.79009</cdr:x>
+      <cdr:y>0.02615</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91883</cdr:x>
+      <cdr:y>0.09621</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DD3E36-EF67-BA1D-5718-79985B13DC6B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5611467" y="129418"/>
+          <a:ext cx="914400" cy="346834"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" kern="1200">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>9950X</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-DK" sz="1600" kern="1200">
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.37231</cdr:x>
+      <cdr:y>0.30623</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.50106</cdr:x>
+      <cdr:y>0.3763</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{961A972F-631D-4A04-BE28-08C45BCA6B10}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2644291" y="1515787"/>
+          <a:ext cx="914400" cy="346834"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" kern="1200">
+              <a:solidFill>
+                <a:srgbClr val="7CAFDE"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>5950X</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-DK" sz="1600" kern="1200">
+            <a:solidFill>
+              <a:srgbClr val="7CAFDE"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -1821,7 +2050,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update graph in Sep 0.10.0 - 21 GB/s CSV Parsing Using SIMD on AMD 9950X 🚀 (#55)
</commit_message>
<xml_diff>
--- a/images/2025-05-sep-0.10.0/sep-perf-0.1.0-to-0.10.0.xlsx
+++ b/images/2025-05-sep-0.10.0/sep-perf-0.1.0-to-0.10.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\oss\nietras.github.io\images\2025-04-sep-0.10.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\oss\nietras.github.io\images\2025-05-sep-0.10.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3CBC92-2054-4A3B-AD46-5311E6513306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACD6FA6-A64A-4EE5-A86D-9257DE07B4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,6 +195,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7CAFDE"/>
       <color rgb="FFC198E0"/>
       <color rgb="FFB482DA"/>
     </mruColors>
@@ -1473,12 +1474,63 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
+      <cdr:x>0.7828</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78499</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA92422-2B5F-8441-9152-04C287BCECF4}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="5559700" y="0"/>
+          <a:ext cx="15530" cy="4949895"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
       <cdr:x>0.29446</cdr:x>
       <cdr:y>0.02196</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.7121</cdr:x>
-      <cdr:y>0.28199</cdr:y>
+      <cdr:y>0.30119</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1493,8 +1545,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2091358" y="108710"/>
-          <a:ext cx="2966210" cy="1287117"/>
+          <a:off x="2091354" y="108700"/>
+          <a:ext cx="2966219" cy="1382170"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1543,9 +1595,186 @@
             </a:rPr>
             <a:t>Performance Progression</a:t>
           </a:r>
-          <a:endParaRPr lang="en-DK" sz="2000" kern="1200">
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C198E0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Across Different Sep &amp; .NET Versions and CPUs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-DK" sz="1100" kern="1200">
             <a:solidFill>
               <a:srgbClr val="C198E0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.79009</cdr:x>
+      <cdr:y>0.02615</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91883</cdr:x>
+      <cdr:y>0.09621</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DD3E36-EF67-BA1D-5718-79985B13DC6B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5611467" y="129418"/>
+          <a:ext cx="914400" cy="346834"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" kern="1200">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>9950X</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-DK" sz="1600" kern="1200">
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.37231</cdr:x>
+      <cdr:y>0.30623</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.50106</cdr:x>
+      <cdr:y>0.3763</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{961A972F-631D-4A04-BE28-08C45BCA6B10}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2644291" y="1515787"/>
+          <a:ext cx="914400" cy="346834"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" kern="1200">
+              <a:solidFill>
+                <a:srgbClr val="7CAFDE"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>5950X</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-DK" sz="1600" kern="1200">
+            <a:solidFill>
+              <a:srgbClr val="7CAFDE"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -1821,7 +2050,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>